<commit_message>
Kenyan Corona Updates as of 5th April 2020
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -185,6 +185,18 @@
   </si>
   <si>
     <t>20 - 67</t>
+  </si>
+  <si>
+    <t>Nigerian(1)</t>
+  </si>
+  <si>
+    <t>Nairobi(12), Kilifi(1),Mombasa(3)</t>
+  </si>
+  <si>
+    <t>22-66</t>
+  </si>
+  <si>
+    <t>Community(5), Imported(11)</t>
   </si>
 </sst>
 </file>
@@ -546,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P22"/>
+  <dimension ref="A2:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +569,7 @@
     <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="23.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
@@ -1251,6 +1263,12 @@
       <c r="G22" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
       <c r="K22" s="1" t="s">
         <v>13</v>
       </c>
@@ -1262,6 +1280,47 @@
       </c>
       <c r="P22" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>43926</v>
+      </c>
+      <c r="B23" s="1">
+        <v>16</v>
+      </c>
+      <c r="C23" s="1">
+        <v>530</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F23" s="1">
+        <v>142</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O23" s="1">
+        <v>7</v>
+      </c>
+      <c r="P23" s="1">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
6th April 2020 Kenya COVID-19 updates
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -558,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P23"/>
+  <dimension ref="A2:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,6 +1326,29 @@
         <v>9</v>
       </c>
     </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>43927</v>
+      </c>
+      <c r="B24" s="1">
+        <v>16</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4277</v>
+      </c>
+      <c r="F24" s="1">
+        <v>158</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1"/>

</xml_diff>

<commit_message>
7th April 2020 Kenya COVID-19 updates
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>Community(5), Imported(11)</t>
+  </si>
+  <si>
+    <t>Community(10),Imported(4)</t>
+  </si>
+  <si>
+    <t>Tanzania, UAE, South Africa, United States</t>
+  </si>
+  <si>
+    <t>Nairobi(7), Mombasa(2), Machakos (1), Kisii(1), Kiambu (1) Mandera (2)</t>
   </si>
 </sst>
 </file>
@@ -558,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P24"/>
+  <dimension ref="A2:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,8 +578,8 @@
     <col min="1" max="1" width="13.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="26.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="36.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="47" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" style="1" customWidth="1"/>
     <col min="8" max="9" width="9.140625" style="1"/>
@@ -1347,6 +1356,38 @@
       </c>
       <c r="K24" s="1" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>43928</v>
+      </c>
+      <c r="B25" s="1">
+        <v>14</v>
+      </c>
+      <c r="C25" s="1">
+        <v>696</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="1">
+        <v>172</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="1">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates as of 8th April 2020
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="67">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -206,6 +206,15 @@
   </si>
   <si>
     <t>Nairobi(7), Mombasa(2), Machakos (1), Kisii(1), Kiambu (1) Mandera (2)</t>
+  </si>
+  <si>
+    <t>Community(4), Imported(3)</t>
+  </si>
+  <si>
+    <t>Congo, United States, UK(2)</t>
+  </si>
+  <si>
+    <t>Nairobi, Mombasa, Uasin Ngishu</t>
   </si>
 </sst>
 </file>
@@ -567,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P25"/>
+  <dimension ref="A2:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1390,6 +1399,38 @@
         <v>13</v>
       </c>
     </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>43929</v>
+      </c>
+      <c r="B26" s="1">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1">
+        <v>305</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F26" s="1">
+        <v>179</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates as of 10th April 2020
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -130,9 +130,6 @@
     <t>United States, Cameroon, Burkina Faso</t>
   </si>
   <si>
-    <t>Nairobi(3), Mombasa (1)</t>
-  </si>
-  <si>
     <t>Male Infected</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>Community (1),Import (3)</t>
   </si>
   <si>
-    <t>Kitui(1),Nairobi(6),Mombasa(1)</t>
-  </si>
-  <si>
     <t>Narobi, Mombasa,Kilifi(5),Kwale</t>
   </si>
   <si>
@@ -239,6 +233,12 @@
   </si>
   <si>
     <t>Community(4), Imported</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nairobi(3), Mombasa </t>
+  </si>
+  <si>
+    <t>Kitui(1),Nairobi(6),Mombasa</t>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
   <dimension ref="A2:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,10 +670,10 @@
         <v>33</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -815,7 +815,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -921,7 +921,7 @@
         <v>13</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -962,7 +962,7 @@
         <v>82</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F12" s="1">
         <v>25</v>
@@ -1026,7 +1026,7 @@
         <v>74</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F14" s="1">
         <v>31</v>
@@ -1102,13 +1102,13 @@
         <v>37</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="F16" s="1">
         <v>42</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H16" s="1">
         <v>0</v>
@@ -1128,7 +1128,7 @@
         <v>172</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="F17" s="1">
         <v>50</v>
@@ -1183,10 +1183,10 @@
         <v>380</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F19" s="1">
         <v>81</v>
@@ -1201,7 +1201,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O19" s="1">
         <v>9</v>
@@ -1221,7 +1221,7 @@
         <v>662</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>16</v>
@@ -1239,13 +1239,13 @@
         <v>2</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="O20" s="1">
         <v>16</v>
@@ -1262,7 +1262,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>16</v>
@@ -1280,7 +1280,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N21" s="1">
         <v>6</v>
@@ -1297,7 +1297,7 @@
         <v>372</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>16</v>
@@ -1318,7 +1318,7 @@
         <v>13</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="O22" s="1">
         <v>1</v>
@@ -1338,16 +1338,16 @@
         <v>530</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F23" s="1">
         <v>142</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
@@ -1359,7 +1359,7 @@
         <v>30</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="O23" s="1">
         <v>7</v>
@@ -1402,16 +1402,16 @@
         <v>696</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F25" s="1">
         <v>172</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H25" s="1">
         <v>3</v>
@@ -1434,16 +1434,16 @@
         <v>305</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F26" s="1">
         <v>179</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H26" s="1">
         <v>0</v>
@@ -1466,16 +1466,16 @@
         <v>308</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F27" s="1">
         <v>184</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H27" s="1">
         <v>4</v>
@@ -1484,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O27" s="1">
         <v>2</v>
@@ -1504,16 +1504,16 @@
         <v>504</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F28" s="1">
         <v>189</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H28" s="1">
         <v>10</v>
@@ -1522,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O28" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
Updates as of 15th April 2020
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -223,9 +223,6 @@
     <t>Nigerian</t>
   </si>
   <si>
-    <t>Spain[2] , Dubai</t>
-  </si>
-  <si>
     <t>Nairobi,Mombasa,Nyandarua(3)</t>
   </si>
   <si>
@@ -239,6 +236,63 @@
   </si>
   <si>
     <t>Kitui(1),Nairobi(6),Mombasa</t>
+  </si>
+  <si>
+    <t>Nairobi,Mombasa</t>
+  </si>
+  <si>
+    <t>Community(2)</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Spain(2) , Dubai</t>
+  </si>
+  <si>
+    <t>02 - 32.</t>
+  </si>
+  <si>
+    <t>Nairobi(4),Mombasa,Siaya</t>
+  </si>
+  <si>
+    <t>UAE(2)</t>
+  </si>
+  <si>
+    <t>25-59</t>
+  </si>
+  <si>
+    <t>Community(4), Imported(2)</t>
+  </si>
+  <si>
+    <t>UAE(4)</t>
+  </si>
+  <si>
+    <t>1-42.</t>
+  </si>
+  <si>
+    <t>Mandera(4),Mombasa(3),Nairobi(2),Nakuru, Machakos</t>
+  </si>
+  <si>
+    <t>Community(7),Imported(4)</t>
+  </si>
+  <si>
+    <t>Community(2), Imported(6)</t>
+  </si>
+  <si>
+    <t>UAE(2),UK,Pakistan,Zambia,Comoros</t>
+  </si>
+  <si>
+    <t>Nairobi(6),Siaya,Nakuru</t>
+  </si>
+  <si>
+    <t>Community(9)</t>
+  </si>
+  <si>
+    <t>Nairobi(5), Mombasa(4)</t>
+  </si>
+  <si>
+    <t>9-69.</t>
   </si>
 </sst>
 </file>
@@ -283,7 +337,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,6 +347,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -600,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P28"/>
+  <dimension ref="A2:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +872,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
@@ -1102,7 +1159,7 @@
         <v>37</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F16" s="1">
         <v>42</v>
@@ -1128,7 +1185,7 @@
         <v>172</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" s="1">
         <v>50</v>
@@ -1414,7 +1471,7 @@
         <v>54</v>
       </c>
       <c r="H25" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -1507,13 +1564,13 @@
         <v>64</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F28" s="1">
         <v>189</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H28" s="1">
         <v>10</v>
@@ -1522,13 +1579,182 @@
         <v>0</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O28" s="1">
         <v>3</v>
       </c>
       <c r="P28" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>43932</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1">
+        <v>491</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="1">
+        <v>191</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="1">
+        <v>2</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="O29" s="1">
+        <v>1</v>
+      </c>
+      <c r="P29" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>43933</v>
+      </c>
+      <c r="B30" s="1">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1">
+        <v>766</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="1">
+        <v>197</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>43934</v>
+      </c>
+      <c r="B31" s="1">
+        <v>11</v>
+      </c>
+      <c r="C31" s="1">
+        <v>674</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="1">
+        <v>208</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H31" s="1">
+        <v>15</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="O31" s="1">
+        <v>5</v>
+      </c>
+      <c r="P31" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>43935</v>
+      </c>
+      <c r="B32" s="1">
+        <v>8</v>
+      </c>
+      <c r="C32" s="1">
+        <v>694</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="1">
+        <v>216</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>43936</v>
+      </c>
+      <c r="B33" s="1">
+        <v>9</v>
+      </c>
+      <c r="C33" s="1">
+        <v>803</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" s="1">
+        <v>225</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H33" s="1">
+        <v>12</v>
+      </c>
+      <c r="I33" s="1">
+        <v>1</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on 16th April 2020
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="94">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>9-69.</t>
+  </si>
+  <si>
+    <t>2-64.</t>
   </si>
 </sst>
 </file>
@@ -657,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P33"/>
+  <dimension ref="A2:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1757,6 +1760,29 @@
         <v>92</v>
       </c>
     </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>43937</v>
+      </c>
+      <c r="B34" s="1">
+        <v>9</v>
+      </c>
+      <c r="C34" s="1">
+        <v>704</v>
+      </c>
+      <c r="F34" s="1">
+        <v>234</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1"/>

</xml_diff>

<commit_message>
Covid-19 Updates 20th April
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="103">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -296,6 +296,33 @@
   </si>
   <si>
     <t>2-64.</t>
+  </si>
+  <si>
+    <t>Community(5)</t>
+  </si>
+  <si>
+    <t>Community(16)</t>
+  </si>
+  <si>
+    <t>Nairobi(9),Mombasa(5), Homabay(1)</t>
+  </si>
+  <si>
+    <t>23-84</t>
+  </si>
+  <si>
+    <t>Community(8)</t>
+  </si>
+  <si>
+    <t>17-65</t>
+  </si>
+  <si>
+    <t>Mombasa(7),Nairobi(4)</t>
+  </si>
+  <si>
+    <t>Community(11)</t>
+  </si>
+  <si>
+    <t>11-80.</t>
   </si>
 </sst>
 </file>
@@ -660,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P34"/>
+  <dimension ref="A2:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,7 +1501,7 @@
         <v>54</v>
       </c>
       <c r="H25" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I25" s="1">
         <v>0</v>
@@ -1728,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>43936</v>
       </c>
@@ -1760,7 +1787,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>43937</v>
       </c>
@@ -1781,6 +1808,122 @@
       </c>
       <c r="L34" s="1" t="s">
         <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B35" s="1">
+        <v>12</v>
+      </c>
+      <c r="C35" s="1">
+        <v>450</v>
+      </c>
+      <c r="F35" s="1">
+        <v>246</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H35" s="1">
+        <v>0</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B36" s="1">
+        <v>16</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1115</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" s="1">
+        <v>262</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" s="1">
+        <v>7</v>
+      </c>
+      <c r="I36" s="1">
+        <v>1</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="O36" s="1">
+        <v>4</v>
+      </c>
+      <c r="P36" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B37" s="1">
+        <v>8</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1330</v>
+      </c>
+      <c r="F37" s="1">
+        <v>270</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H37" s="1">
+        <v>7</v>
+      </c>
+      <c r="I37" s="1">
+        <v>2</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B38" s="1">
+        <v>11</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F38" s="1">
+        <v>281</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H38" s="1">
+        <v>2</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="O38" s="1">
+        <v>6</v>
+      </c>
+      <c r="P38" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates on Corona Virus in Kenya on 21st April
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="106">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -323,6 +323,15 @@
   </si>
   <si>
     <t>11-80.</t>
+  </si>
+  <si>
+    <t>Mombasa(7),Nairobi(6),Mandera(2)</t>
+  </si>
+  <si>
+    <t>Community(15)</t>
+  </si>
+  <si>
+    <t>19-75</t>
   </si>
 </sst>
 </file>
@@ -687,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P38"/>
+  <dimension ref="A2:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="E18" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,14 +1925,58 @@
       <c r="I38" s="1">
         <v>0</v>
       </c>
+      <c r="K38" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="L38" s="5" t="s">
         <v>102</v>
       </c>
       <c r="O38" s="1">
+        <v>5</v>
+      </c>
+      <c r="P38" s="1">
         <v>6</v>
       </c>
-      <c r="P38" s="1">
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B39" s="1">
+        <v>15</v>
+      </c>
+      <c r="C39" s="1">
+        <v>545</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F39" s="1">
+        <v>296</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H39" s="1">
         <v>5</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O39" s="1">
+        <v>8</v>
+      </c>
+      <c r="P39" s="1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
covid-19 updates as of 22-April-2020
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="107">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -332,6 +332,9 @@
   </si>
   <si>
     <t>19-75</t>
+  </si>
+  <si>
+    <t>Community(7)</t>
   </si>
 </sst>
 </file>
@@ -696,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P39"/>
+  <dimension ref="A2:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E18" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1979,6 +1982,23 @@
         <v>7</v>
       </c>
     </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>43943</v>
+      </c>
+      <c r="B40" s="1">
+        <v>7</v>
+      </c>
+      <c r="C40" s="1">
+        <v>707</v>
+      </c>
+      <c r="F40" s="1">
+        <v>303</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates on Covid-19 on 23rd April 2020
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="109">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -335,6 +335,12 @@
   </si>
   <si>
     <t>Community(7)</t>
+  </si>
+  <si>
+    <t>Mombasa(12),Nairobi(3)</t>
+  </si>
+  <si>
+    <t>Community(17)</t>
   </si>
 </sst>
 </file>
@@ -699,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P40"/>
+  <dimension ref="A2:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="E18" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1998,6 +2004,44 @@
       <c r="G40" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="H40" s="1">
+        <v>0</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>43944</v>
+      </c>
+      <c r="B41" s="1">
+        <v>17</v>
+      </c>
+      <c r="C41" s="1">
+        <v>668</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F41" s="1">
+        <v>320</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Updates on COvid-19 in Kenya 24 April 2020
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -341,6 +341,9 @@
   </si>
   <si>
     <t>Mombasa(12),Nairobi(5)</t>
+  </si>
+  <si>
+    <t>Mombasa(5),Nairobi(11)</t>
   </si>
 </sst>
 </file>
@@ -705,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P41"/>
+  <dimension ref="A2:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E20" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2043,6 +2046,35 @@
         <v>30</v>
       </c>
     </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>43945</v>
+      </c>
+      <c r="B42" s="1">
+        <v>16</v>
+      </c>
+      <c r="C42" s="1">
+        <v>946</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F42" s="1">
+        <v>336</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H42" s="1">
+        <v>5</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates as of 28th April 2020
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -344,6 +344,27 @@
   </si>
   <si>
     <t>Mombasa(5),Nairobi(11)</t>
+  </si>
+  <si>
+    <t>Mombasa(4),Nairobi(7)</t>
+  </si>
+  <si>
+    <t>3-75.</t>
+  </si>
+  <si>
+    <t>14-60</t>
+  </si>
+  <si>
+    <t>Mombasa(4),Nairobi(8)</t>
+  </si>
+  <si>
+    <t>Community(12)</t>
+  </si>
+  <si>
+    <t>13-65</t>
+  </si>
+  <si>
+    <t>Mombasa(4),Nairobi(3),Kwale(1)</t>
   </si>
 </sst>
 </file>
@@ -708,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P42"/>
+  <dimension ref="A2:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2001,6 +2022,9 @@
       <c r="C40" s="1">
         <v>707</v>
       </c>
+      <c r="D40" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="F40" s="1">
         <v>303</v>
       </c>
@@ -2073,6 +2097,122 @@
       </c>
       <c r="I42" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>43946</v>
+      </c>
+      <c r="B43" s="1">
+        <v>7</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F43" s="1">
+        <v>343</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H43" s="1">
+        <v>0</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>43947</v>
+      </c>
+      <c r="B44" s="1">
+        <v>12</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F44" s="1">
+        <v>355</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H44" s="1">
+        <v>8</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>43948</v>
+      </c>
+      <c r="B45" s="1">
+        <v>8</v>
+      </c>
+      <c r="C45" s="1">
+        <v>366</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F45" s="1">
+        <v>363</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H45" s="1">
+        <v>0</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>43949</v>
+      </c>
+      <c r="B46" s="1">
+        <v>11</v>
+      </c>
+      <c r="C46" s="1">
+        <v>579</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F46" s="1">
+        <v>374</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H46" s="1">
+        <v>10</v>
+      </c>
+      <c r="I46" s="1">
+        <v>0</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Covid-19 Kenyan Updates as of 29th April 2020
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="119">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -365,6 +365,12 @@
   </si>
   <si>
     <t>Mombasa(4),Nairobi(3),Kwale(1)</t>
+  </si>
+  <si>
+    <t>Mombasa(9),Nairobi(1)</t>
+  </si>
+  <si>
+    <t>Community(10)</t>
   </si>
 </sst>
 </file>
@@ -729,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P46"/>
+  <dimension ref="A2:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="F23" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2215,6 +2221,44 @@
         <v>111</v>
       </c>
     </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>43950</v>
+      </c>
+      <c r="B47" s="1">
+        <v>10</v>
+      </c>
+      <c r="C47" s="1">
+        <v>508</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F47" s="1">
+        <v>384</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H47" s="1">
+        <v>5</v>
+      </c>
+      <c r="I47" s="1">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O47" s="1">
+        <v>4</v>
+      </c>
+      <c r="P47" s="1">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1"/>

</xml_diff>

<commit_message>
Updates on Covid-19 cases in Kenya as of 30th April 2020
</commit_message>
<xml_diff>
--- a/corona-virus-kenya.xlsx
+++ b/corona-virus-kenya.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="122">
   <si>
     <t xml:space="preserve">Date </t>
   </si>
@@ -371,6 +371,15 @@
   </si>
   <si>
     <t>Community(10)</t>
+  </si>
+  <si>
+    <t>Mombasa(7),Nairobi(5)</t>
+  </si>
+  <si>
+    <t>1-75.</t>
+  </si>
+  <si>
+    <t>Aman</t>
   </si>
 </sst>
 </file>
@@ -735,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P47"/>
+  <dimension ref="A2:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F23" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" topLeftCell="F35" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,6 +2268,47 @@
         <v>6</v>
       </c>
     </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>43951</v>
+      </c>
+      <c r="B48" s="1">
+        <v>12</v>
+      </c>
+      <c r="C48" s="1">
+        <v>777</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F48" s="1">
+        <v>396</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H48" s="1">
+        <v>15</v>
+      </c>
+      <c r="I48" s="1">
+        <v>2</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O48" s="1">
+        <v>3</v>
+      </c>
+      <c r="P48" s="1">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J6" r:id="rId1"/>

</xml_diff>